<commit_message>
Added Calculations for TAX and ETS
</commit_message>
<xml_diff>
--- a/data/ICAOPrefix.xlsx
+++ b/data/ICAOPrefix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D71332B-316C-43F6-80DB-7CEAE318F463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1054EBFA-2B44-41CC-BF82-6A352669E07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="1815" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1738,7 +1738,7 @@
     <t>Canary Islands</t>
   </si>
   <si>
-    <t>Guadeloupe, Martinique, Saint Barthélemy, Saint Martin</t>
+    <t>West Indies</t>
   </si>
 </sst>
 </file>
@@ -2107,7 +2107,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="B259" sqref="B259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6464,7 +6464,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>365</v>
       </c>

</xml_diff>

<commit_message>
Fixed a number of bugs on input fields calculate total fuel req per year Include close outermost regions in GDP calculations added groupping options, not implemented yet added year and gdp growth rate input field for gdp estimation in the future added gmail link added Eurocontrol disclaimer added google analytics
</commit_message>
<xml_diff>
--- a/data/ICAOPrefix.xlsx
+++ b/data/ICAOPrefix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\FuelCost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1054EBFA-2B44-41CC-BF82-6A352669E07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84F1672-C83F-4F62-8DFE-750CD5D035E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
+    <workbookView xWindow="0" yWindow="5595" windowWidth="28800" windowHeight="15555" xr2:uid="{84504369-7A79-4CE5-B3C2-F56AC7F0264A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1720,9 +1720,6 @@
     <t>France</t>
   </si>
   <si>
-    <t xml:space="preserve">Spain </t>
-  </si>
-  <si>
     <t>Italy</t>
   </si>
   <si>
@@ -1739,6 +1736,9 @@
   </si>
   <si>
     <t>West Indies</t>
+  </si>
+  <si>
+    <t>Spain</t>
   </si>
 </sst>
 </file>
@@ -2107,7 +2107,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B259" sqref="B259"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,7 +2232,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>179</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>156</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>160</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>158</v>
       </c>
@@ -2600,12 +2600,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C22" t="s">
         <v>465</v>
@@ -2623,7 +2623,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>171</v>
       </c>
@@ -2646,12 +2646,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C24" t="s">
         <v>456</v>
@@ -2669,7 +2669,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>163</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>164</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>166</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -3428,12 +3428,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C58" t="s">
         <v>465</v>
@@ -4003,7 +4003,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>42</v>
       </c>
@@ -4026,12 +4026,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C84" t="s">
         <v>456</v>
@@ -4049,7 +4049,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>54</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>56</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>45</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>175</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>40</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>47</v>
       </c>
@@ -4187,7 +4187,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>49</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>181</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>184</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>200</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>169</v>
       </c>
@@ -4371,12 +4371,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="C99" t="s">
         <v>456</v>
@@ -4394,7 +4394,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>51</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>186</v>
       </c>
@@ -6234,12 +6234,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>346</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C180" t="s">
         <v>465</v>
@@ -6464,12 +6464,12 @@
         <v>465</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>365</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C190" t="s">
         <v>465</v>
@@ -7614,7 +7614,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>473</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>477</v>
       </c>
@@ -7660,7 +7660,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>478</v>
       </c>
@@ -7683,7 +7683,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>480</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>481</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>482</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>483</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>484</v>
       </c>
@@ -7798,7 +7798,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>485</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>486</v>
       </c>
@@ -7844,7 +7844,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>487</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>488</v>
       </c>
@@ -7890,7 +7890,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>489</v>
       </c>
@@ -7913,7 +7913,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>491</v>
       </c>
@@ -7936,7 +7936,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>487</v>
       </c>
@@ -7970,7 +7970,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G254" xr:uid="{90F610DA-8A3C-41D3-A04E-01BF26B8D586}">
-    <filterColumn colId="4">
+    <filterColumn colId="5">
       <filters>
         <filter val="Y"/>
       </filters>

</xml_diff>